<commit_message>
Cambios en programa de pyton
</commit_message>
<xml_diff>
--- a/Estados y transiciones.xlsx
+++ b/Estados y transiciones.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ac0b2ee2496a8036/Documentos/A01712114/Semestre 4/E2_gramatica/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="264" documentId="8_{77FA31C9-11FC-4A6A-BCCA-CD18D308CA33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D93124D7-2E59-425F-A1ED-3FB26A157600}"/>
+  <xr:revisionPtr revIDLastSave="266" documentId="8_{77FA31C9-11FC-4A6A-BCCA-CD18D308CA33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5651D2E3-35B6-47BD-BD37-C664FBE0590D}"/>
   <bookViews>
-    <workbookView xWindow="9636" yWindow="996" windowWidth="14832" windowHeight="8880" xr2:uid="{DBBA14C6-DE78-4573-92DD-54D8C1744A7F}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="19992" windowHeight="12456" xr2:uid="{DBBA14C6-DE78-4573-92DD-54D8C1744A7F}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -755,7 +755,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24E69366-1E53-49CB-9877-070F18C35348}">
   <dimension ref="B3:AP15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AI1" zoomScale="54" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="32" workbookViewId="0">
       <selection activeCell="AP13" sqref="AP13"/>
     </sheetView>
   </sheetViews>
@@ -772,8 +772,8 @@
     <col min="19" max="19" width="15.109375" customWidth="1"/>
     <col min="20" max="20" width="14.6640625" customWidth="1"/>
     <col min="21" max="21" width="14.77734375" customWidth="1"/>
-    <col min="22" max="22" width="14.5546875" customWidth="1"/>
-    <col min="23" max="23" width="14.88671875" customWidth="1"/>
+    <col min="22" max="22" width="16.6640625" customWidth="1"/>
+    <col min="23" max="23" width="15.5546875" customWidth="1"/>
     <col min="24" max="24" width="13.77734375" customWidth="1"/>
     <col min="25" max="25" width="16" customWidth="1"/>
     <col min="26" max="26" width="13.21875" customWidth="1"/>

</xml_diff>